<commit_message>
Commit via Qualitia by Rohit.Patil
</commit_message>
<xml_diff>
--- a/Web3_projectdb/TestCases/Tc16.xlsx
+++ b/Web3_projectdb/TestCases/Tc16.xlsx
@@ -19,12 +19,6 @@
     <t/>
   </si>
   <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>$NULL$</t>
-  </si>
-  <si>
     <t>Selection</t>
   </si>
   <si>
@@ -34,7 +28,13 @@
     <t>TCIteration</t>
   </si>
   <si>
+    <t>aaa</t>
+  </si>
+  <si>
     <t>key</t>
+  </si>
+  <si>
+    <t>dd</t>
   </si>
   <si>
     <t>True</t>
@@ -781,19 +781,19 @@
     </row>
     <row r="2" ht="25" customHeight="1">
       <c r="A2" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>6</v>
-      </c>
       <c r="E2" s="14" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" ht="25" customHeight="1">
@@ -807,10 +807,10 @@
         <v>0</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E3" s="15" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" ht="25" customHeight="1" s="4" customFormat="1">

</xml_diff>